<commit_message>
Pronto para ir para producao com bolao
.
</commit_message>
<xml_diff>
--- a/Futebol Americano/LFFA/Banco de Dados/tabela.xlsx
+++ b/Futebol Americano/LFFA/Banco de Dados/tabela.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12195"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Usuarios" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="205">
   <si>
     <t>AALD</t>
   </si>
@@ -261,189 +261,6 @@
     <t>);</t>
   </si>
   <si>
-    <t>Vila</t>
-  </si>
-  <si>
-    <t>vila.jpg</t>
-  </si>
-  <si>
-    <t>João Celson</t>
-  </si>
-  <si>
-    <t>Contato para marcar jogos: (32) 984224005</t>
-  </si>
-  <si>
-    <t>32 984224005</t>
-  </si>
-  <si>
-    <t>1964-07-04 00:00:00.000</t>
-  </si>
-  <si>
-    <t>Cruzeiro</t>
-  </si>
-  <si>
-    <t>cruzeiro.jpg</t>
-  </si>
-  <si>
-    <t>Edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contato para marcar jogos: </t>
-  </si>
-  <si>
-    <t>Minas</t>
-  </si>
-  <si>
-    <t>minas.jpg</t>
-  </si>
-  <si>
-    <t>Paulo Cezar</t>
-  </si>
-  <si>
-    <t>aald.jpg</t>
-  </si>
-  <si>
-    <t>Moacir</t>
-  </si>
-  <si>
-    <t>Santa Terezinha</t>
-  </si>
-  <si>
-    <t>santaterezinha.jpg</t>
-  </si>
-  <si>
-    <t>Cléber</t>
-  </si>
-  <si>
-    <t>Esplanado</t>
-  </si>
-  <si>
-    <t>esplanado.jpg</t>
-  </si>
-  <si>
-    <t>Geraldo Fonseca</t>
-  </si>
-  <si>
-    <t>Juventus</t>
-  </si>
-  <si>
-    <t>juventus.jpg</t>
-  </si>
-  <si>
-    <t>Samuel</t>
-  </si>
-  <si>
-    <t>Vila Santo Antônio</t>
-  </si>
-  <si>
-    <t>santoantonio.jpg</t>
-  </si>
-  <si>
-    <t>Robertinho</t>
-  </si>
-  <si>
-    <t>Bahia</t>
-  </si>
-  <si>
-    <t>bahia.jpg</t>
-  </si>
-  <si>
-    <t>Apagao</t>
-  </si>
-  <si>
-    <t>Apagao.jpg</t>
-  </si>
-  <si>
-    <t>Caete</t>
-  </si>
-  <si>
-    <t>Caete.jpg</t>
-  </si>
-  <si>
-    <t>Manejo</t>
-  </si>
-  <si>
-    <t>Manejo.jpg</t>
-  </si>
-  <si>
-    <t>Laranjeira</t>
-  </si>
-  <si>
-    <t>Laranjeira.jpg</t>
-  </si>
-  <si>
-    <t>Ipiranga</t>
-  </si>
-  <si>
-    <t>Ipiranga.jpg</t>
-  </si>
-  <si>
-    <t>Vila Sao Geraldo</t>
-  </si>
-  <si>
-    <t>vsgfc.jpg</t>
-  </si>
-  <si>
-    <t>Rosa Gomes</t>
-  </si>
-  <si>
-    <t>rosagomes.jpg</t>
-  </si>
-  <si>
-    <t>Juventude</t>
-  </si>
-  <si>
-    <t>juventude.jpg</t>
-  </si>
-  <si>
-    <t>São Domingos</t>
-  </si>
-  <si>
-    <t>saodomingos.jpg</t>
-  </si>
-  <si>
-    <t>Perobas</t>
-  </si>
-  <si>
-    <t>perobas.jpg</t>
-  </si>
-  <si>
-    <t>Serab</t>
-  </si>
-  <si>
-    <t>serab.jpg</t>
-  </si>
-  <si>
-    <t>Social</t>
-  </si>
-  <si>
-    <t>social.jpg</t>
-  </si>
-  <si>
-    <t>Poço da Pedra</t>
-  </si>
-  <si>
-    <t>pocopedra.jpg</t>
-  </si>
-  <si>
-    <t>Polemica</t>
-  </si>
-  <si>
-    <t>polemica.jpg</t>
-  </si>
-  <si>
-    <t>Piuna</t>
-  </si>
-  <si>
-    <t>piuna.jpg</t>
-  </si>
-  <si>
-    <t>Orvalho</t>
-  </si>
-  <si>
-    <t>orvalho.jpg</t>
-  </si>
-  <si>
     <t>JUIZ DE FORA</t>
   </si>
   <si>
@@ -685,6 +502,135 @@
   </si>
   <si>
     <t>Hunters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mamutes </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Laércio Azalim Júnior</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Red fox </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Matheus Locke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Angra Destroyes </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mychel Reis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Blaze </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Diego Braga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hunter </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rafael Melo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gaditas </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rodrigo Oliveira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Shadows </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wlad Barbosa</t>
+  </si>
+  <si>
+    <t>insert into usuario (</t>
+  </si>
+  <si>
+    <t>Laercio Azalim Júnior</t>
+  </si>
+  <si>
+    <t>mamutes02</t>
+  </si>
+  <si>
+    <t>laercio.azalim@gmail.com</t>
+  </si>
+  <si>
+    <t>Matheus Locke</t>
+  </si>
+  <si>
+    <t>redfox22</t>
+  </si>
+  <si>
+    <t>matheus.locke</t>
+  </si>
+  <si>
+    <t>Mychel Reis</t>
+  </si>
+  <si>
+    <t>destroyes43</t>
+  </si>
+  <si>
+    <t>mychel.reis@gmail.com</t>
+  </si>
+  <si>
+    <t>Diego Braga</t>
+  </si>
+  <si>
+    <t>blaze32</t>
+  </si>
+  <si>
+    <t>diego.braga@gmail.com</t>
+  </si>
+  <si>
+    <t>Rafael Melo</t>
+  </si>
+  <si>
+    <t>hunter43</t>
+  </si>
+  <si>
+    <t>rafael.melo@gmail.com</t>
+  </si>
+  <si>
+    <t>Rodrigo Oliveira</t>
+  </si>
+  <si>
+    <t>gaditas76</t>
+  </si>
+  <si>
+    <t>rodrigo.oliveira@gmail.com</t>
+  </si>
+  <si>
+    <t>Wlad Barbosa</t>
+  </si>
+  <si>
+    <t>shadows54</t>
+  </si>
+  <si>
+    <t>wlad.barbosa@gmail.com</t>
+  </si>
+  <si>
+    <t>Comentarista Partida</t>
+  </si>
+  <si>
+    <t>liffa2016</t>
+  </si>
+  <si>
+    <t>narrador.liffa@gmail.com</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Senha</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="T17" sqref="N15:T17"/>
     </sheetView>
   </sheetViews>
@@ -1085,20 +1031,20 @@
         <v>42463</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D2" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>216</v>
+        <v>155</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
@@ -1110,7 +1056,7 @@
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>15</v>
@@ -1128,7 +1074,7 @@
         <v>14</v>
       </c>
       <c r="R2" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>16</v>
@@ -1148,20 +1094,20 @@
         <v>42463</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>217</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
@@ -1173,7 +1119,7 @@
         <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>15</v>
@@ -1191,7 +1137,7 @@
         <v>14</v>
       </c>
       <c r="R3" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>16</v>
@@ -1211,20 +1157,20 @@
         <v>42470</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="D4" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>218</v>
+        <v>157</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
@@ -1236,7 +1182,7 @@
         <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>167</v>
+        <v>106</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>15</v>
@@ -1254,7 +1200,7 @@
         <v>14</v>
       </c>
       <c r="R4" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>16</v>
@@ -1274,20 +1220,20 @@
         <v>42484</v>
       </c>
       <c r="C5" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="D5" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>88</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>219</v>
+        <v>158</v>
       </c>
       <c r="I5" t="s">
         <v>12</v>
@@ -1317,7 +1263,7 @@
         <v>14</v>
       </c>
       <c r="R5" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>16</v>
@@ -1337,20 +1283,20 @@
         <v>42491</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="D6" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E6" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>220</v>
+        <v>159</v>
       </c>
       <c r="I6" t="s">
         <v>12</v>
@@ -1380,7 +1326,7 @@
         <v>14</v>
       </c>
       <c r="R6" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>16</v>
@@ -1400,20 +1346,20 @@
         <v>42498</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D7" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>221</v>
+        <v>160</v>
       </c>
       <c r="I7" t="s">
         <v>12</v>
@@ -1425,7 +1371,7 @@
         <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>168</v>
+        <v>107</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>15</v>
@@ -1443,7 +1389,7 @@
         <v>14</v>
       </c>
       <c r="R7" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>16</v>
@@ -1463,20 +1409,20 @@
         <v>42512</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E8" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>222</v>
+        <v>161</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
@@ -1488,7 +1434,7 @@
         <v>14</v>
       </c>
       <c r="L8" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>15</v>
@@ -1506,7 +1452,7 @@
         <v>14</v>
       </c>
       <c r="R8" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="S8" s="4" t="s">
         <v>16</v>
@@ -1526,13 +1472,13 @@
         <v>42512</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="D9" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E9" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="F9" s="2"/>
       <c r="I9" t="s">
@@ -1545,7 +1491,7 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>15</v>
@@ -1563,7 +1509,7 @@
         <v>14</v>
       </c>
       <c r="R9" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>16</v>
@@ -1583,13 +1529,13 @@
         <v>42526</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>94</v>
       </c>
       <c r="F10" s="2"/>
       <c r="I10" t="s">
@@ -1602,7 +1548,7 @@
         <v>14</v>
       </c>
       <c r="L10" t="s">
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>15</v>
@@ -1620,7 +1566,7 @@
         <v>14</v>
       </c>
       <c r="R10" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>16</v>
@@ -1640,13 +1586,13 @@
         <v>42526</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="D11" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E11" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
       <c r="F11" s="2"/>
       <c r="I11" t="s">
@@ -1659,7 +1605,7 @@
         <v>14</v>
       </c>
       <c r="L11" t="s">
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>15</v>
@@ -1677,7 +1623,7 @@
         <v>14</v>
       </c>
       <c r="R11" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>16</v>
@@ -1697,13 +1643,13 @@
         <v>42540</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>96</v>
       </c>
       <c r="D12" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E12" t="s">
-        <v>158</v>
+        <v>97</v>
       </c>
       <c r="F12" s="2"/>
       <c r="I12" t="s">
@@ -1716,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="L12" t="s">
-        <v>171</v>
+        <v>110</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>15</v>
@@ -1734,7 +1680,7 @@
         <v>14</v>
       </c>
       <c r="R12" t="s">
-        <v>157</v>
+        <v>96</v>
       </c>
       <c r="S12" s="4" t="s">
         <v>16</v>
@@ -1754,13 +1700,13 @@
         <v>42547</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D13" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>98</v>
       </c>
       <c r="F13" s="2"/>
       <c r="I13" t="s">
@@ -1773,7 +1719,7 @@
         <v>14</v>
       </c>
       <c r="L13" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>15</v>
@@ -1791,7 +1737,7 @@
         <v>14</v>
       </c>
       <c r="R13" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="S13" s="4" t="s">
         <v>16</v>
@@ -1811,13 +1757,13 @@
         <v>42547</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D14" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E14" t="s">
-        <v>160</v>
+        <v>99</v>
       </c>
       <c r="F14" s="2"/>
       <c r="I14" t="s">
@@ -1830,7 +1776,7 @@
         <v>14</v>
       </c>
       <c r="L14" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>15</v>
@@ -1848,7 +1794,7 @@
         <v>14</v>
       </c>
       <c r="R14" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="S14" s="4" t="s">
         <v>16</v>
@@ -1868,13 +1814,13 @@
         <v>42568</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="D15" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
       <c r="F15" s="2"/>
       <c r="M15" s="4"/>
@@ -1891,13 +1837,13 @@
         <v>42568</v>
       </c>
       <c r="C16" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="D16" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E16" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
       <c r="F16" s="2"/>
       <c r="M16" s="4"/>
@@ -1914,13 +1860,13 @@
         <v>42582</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>103</v>
       </c>
       <c r="D17" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E17" t="s">
-        <v>165</v>
+        <v>104</v>
       </c>
       <c r="F17" s="2"/>
       <c r="M17" s="4"/>
@@ -1955,13 +1901,13 @@
     </row>
     <row r="21" spans="1:21">
       <c r="B21" s="1" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>174</v>
+        <v>113</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>175</v>
+        <v>114</v>
       </c>
       <c r="F21" s="2"/>
       <c r="M21" s="4"/>
@@ -1970,23 +1916,23 @@
     </row>
     <row r="22" spans="1:21">
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>176</v>
+        <v>115</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>177</v>
+        <v>116</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="H22" t="s">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="I22" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="M22" s="4"/>
       <c r="S22" s="4"/>
@@ -1994,23 +1940,23 @@
     </row>
     <row r="23" spans="1:21">
       <c r="B23" s="1" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C23" t="s">
-        <v>178</v>
+        <v>117</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>179</v>
+        <v>118</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="H23" t="s">
-        <v>190</v>
+        <v>129</v>
       </c>
       <c r="I23" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="M23" s="4"/>
       <c r="S23" s="4"/>
@@ -2018,23 +1964,23 @@
     </row>
     <row r="24" spans="1:21">
       <c r="B24" s="1" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>181</v>
+        <v>120</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="H24" t="s">
-        <v>191</v>
+        <v>130</v>
       </c>
       <c r="I24" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="M24" s="4"/>
       <c r="S24" s="4"/>
@@ -2042,23 +1988,23 @@
     </row>
     <row r="25" spans="1:21">
       <c r="B25" s="1" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>183</v>
+        <v>122</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="H25" t="s">
-        <v>192</v>
+        <v>131</v>
       </c>
       <c r="I25" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="M25" s="4"/>
       <c r="S25" s="4"/>
@@ -2066,23 +2012,23 @@
     </row>
     <row r="26" spans="1:21">
       <c r="B26" s="1" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="H26" t="s">
-        <v>193</v>
+        <v>132</v>
       </c>
       <c r="I26" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="M26" s="4"/>
       <c r="S26" s="4"/>
@@ -2090,23 +2036,23 @@
     </row>
     <row r="27" spans="1:21">
       <c r="B27" s="1" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C27" t="s">
-        <v>186</v>
+        <v>125</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>181</v>
+        <v>120</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="3" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="H27" t="s">
-        <v>194</v>
+        <v>133</v>
       </c>
       <c r="I27" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="M27" s="4"/>
       <c r="S27" s="4"/>
@@ -2117,13 +2063,13 @@
       <c r="D28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="3" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="H28" t="s">
-        <v>195</v>
+        <v>134</v>
       </c>
       <c r="I28" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="M28" s="4"/>
       <c r="S28" s="4"/>
@@ -4034,13 +3980,13 @@
         <v>42463</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D8" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E8" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -4051,13 +3997,13 @@
         <v>42463</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4068,13 +4014,13 @@
         <v>42470</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4085,13 +4031,13 @@
         <v>42484</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="D11" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E11" t="s">
-        <v>149</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -4102,13 +4048,13 @@
         <v>42491</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="D12" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E12" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -4119,13 +4065,13 @@
         <v>42498</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D13" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4136,13 +4082,13 @@
         <v>42512</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="D14" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E14" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -4153,13 +4099,13 @@
         <v>42512</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E15" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4170,13 +4116,13 @@
         <v>42526</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -4187,13 +4133,13 @@
         <v>42526</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E17" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4204,13 +4150,13 @@
         <v>42540</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>96</v>
       </c>
       <c r="D18" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4221,13 +4167,13 @@
         <v>42547</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D19" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E19" t="s">
-        <v>159</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -4238,13 +4184,13 @@
         <v>42547</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E20" t="s">
-        <v>160</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -4255,13 +4201,13 @@
         <v>42568</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="D21" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E21" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -4272,13 +4218,13 @@
         <v>42568</v>
       </c>
       <c r="C22" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="D22" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E22" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -4289,92 +4235,92 @@
         <v>42582</v>
       </c>
       <c r="C23" t="s">
-        <v>164</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="E23" t="s">
-        <v>165</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B34" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4398,86 +4344,86 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B43" t="s">
-        <v>200</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B44" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B45" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B48" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>206</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -4501,86 +4447,86 @@
         <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>208</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B55" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B56" t="s">
-        <v>200</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B57" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B58" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B59" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B61" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>206</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -4604,91 +4550,91 @@
         <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>209</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
-        <v>200</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B72" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B73" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B74" t="s">
-        <v>206</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -4712,91 +4658,91 @@
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>212</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B80" t="s">
-        <v>200</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B81" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B82" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B83" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B84" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B85" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B86" t="s">
-        <v>206</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -4820,91 +4766,91 @@
         <v>1</v>
       </c>
       <c r="I87" t="s">
-        <v>213</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B91" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B92" t="s">
-        <v>200</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B93" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B94" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B95" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B96" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B97" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B98" t="s">
-        <v>206</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4928,91 +4874,91 @@
         <v>1</v>
       </c>
       <c r="I99" t="s">
-        <v>214</v>
+        <v>153</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B103" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B104" t="s">
-        <v>200</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B106" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B107" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B108" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B109" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="B110" t="s">
-        <v>206</v>
+        <v>145</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -5036,7 +4982,7 @@
         <v>1</v>
       </c>
       <c r="I111" t="s">
-        <v>215</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -5046,467 +4992,208 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
+      <c r="B14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+      <c r="B15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="B16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
+      <c r="B17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
+      <c r="B18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
+      <c r="B19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
+      <c r="B20" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" t="s">
-        <v>119</v>
-      </c>
-      <c r="E14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C17" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" t="s">
-        <v>127</v>
-      </c>
-      <c r="E18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" t="s">
-        <v>129</v>
-      </c>
-      <c r="E19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" t="s">
-        <v>131</v>
-      </c>
-      <c r="E20" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21">
-        <v>23</v>
-      </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>199</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23">
-        <v>25</v>
-      </c>
-      <c r="B23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" t="s">
-        <v>137</v>
-      </c>
-      <c r="E23" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25">
-        <v>27</v>
-      </c>
-      <c r="B25" t="s">
-        <v>140</v>
-      </c>
-      <c r="C25" t="s">
-        <v>141</v>
-      </c>
-      <c r="E25" t="s">
-        <v>90</v>
-      </c>
-      <c r="G25" t="s">
-        <v>86</v>
+        <v>200</v>
+      </c>
+      <c r="D21" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>